<commit_message>
Add SQL script to identify employees attending all company events
</commit_message>
<xml_diff>
--- a/Employee_Attending_Events/Problem_Statement.xlsx
+++ b/Employee_Attending_Events/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q18/Video_Q18_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Employee_Attending_Events\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E452441C-415C-534E-939C-8179730360ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76160294-D406-45EF-8067-2901AEB938F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{6E5816C5-57E1-C048-9AF1-18928797CEBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{6E5816C5-57E1-C048-9AF1-18928797CEBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -87,9 +85,6 @@
   </si>
   <si>
     <t>OUTPUT</t>
-  </si>
-  <si>
-    <t>Video #18 - Employee attending all events</t>
   </si>
   <si>
     <r>
@@ -113,6 +108,9 @@
       <t xml:space="preserve">
 Find out the employees who attended all the company events.</t>
     </r>
+  </si>
+  <si>
+    <t># - Employee attending all events</t>
   </si>
 </sst>
 </file>
@@ -485,6 +483,14 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,14 +514,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,78 +851,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F474954-52E7-9C4B-B770-BFB9DEB6AC98}">
   <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="10" width="18.83203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="8.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" style="1"/>
+    <col min="5" max="5" width="15.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" style="1"/>
+    <col min="9" max="10" width="18.796875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="2:10" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="B1" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+    </row>
+    <row r="2" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-    </row>
-    <row r="2" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-    </row>
-    <row r="5" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+    </row>
+    <row r="3" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="5" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="E6" s="24" t="s">
+      <c r="C6" s="30"/>
+      <c r="E6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="I6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
         <v>7</v>
       </c>
@@ -947,7 +945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -963,14 +961,14 @@
       <c r="G8" s="14">
         <v>45352</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>2</v>
       </c>
@@ -986,14 +984,14 @@
       <c r="G9" s="17">
         <v>45352</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="27">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <v>3</v>
       </c>
@@ -1010,7 +1008,7 @@
         <v>45352</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="10">
         <v>4</v>
       </c>
@@ -1027,7 +1025,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E12" s="15" t="s">
         <v>5</v>
       </c>
@@ -1038,7 +1036,7 @@
         <v>45354</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E13" s="15" t="s">
         <v>5</v>
       </c>
@@ -1049,7 +1047,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E14" s="15" t="s">
         <v>5</v>
       </c>
@@ -1060,7 +1058,7 @@
         <v>45353</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E15" s="15" t="s">
         <v>6</v>
       </c>
@@ -1071,7 +1069,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E16" s="15" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1080,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E17" s="15" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>45355</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E18" s="18" t="s">
         <v>6</v>
       </c>

</xml_diff>